<commit_message>
ERR Advance Payment updates
</commit_message>
<xml_diff>
--- a/PIT3/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT3/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF1FBC3D-50AB-466F-8EDB-FD1064147B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC6B4A-309D-4B0B-A7AF-D6D04101D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27960" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="193">
   <si>
     <t xml:space="preserve">Latest Version History </t>
   </si>
@@ -603,12 +603,39 @@
   <si>
     <t>77, 105, 4, 55, 65, 75, 116, 117, 118, 119, 121</t>
   </si>
+  <si>
+    <t>Advance payment reconciliation reported in error</t>
+  </si>
+  <si>
+    <t>Advance Payment Reconciliation not to be reported with this category or sub-category.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advance Payment reconciliation </t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided.</t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided due to RPN service error.</t>
+  </si>
+  <si>
+    <t>EmployerRegistrationId</t>
+  </si>
+  <si>
+    <t>173, 174</t>
+  </si>
+  <si>
+    <t>Added rules</t>
+  </si>
+  <si>
+    <t>Removed 173</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,8 +744,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,8 +810,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -891,13 +942,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1111,6 +1193,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1149,6 +1270,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -21849,8 +21982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B8:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21865,18 +21998,18 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -21917,7 +22050,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="76">
+      <c r="B14" s="89">
         <v>0.12</v>
       </c>
       <c r="C14" s="71">
@@ -21926,49 +22059,49 @@
       <c r="D14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="79">
+      <c r="E14" s="92">
         <v>45218</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="77"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="34" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="80"/>
+      <c r="E15" s="93"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="77"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="93"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="71" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="80"/>
+      <c r="E17" s="93"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="78"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="81"/>
+      <c r="E18" s="94"/>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="59">
@@ -21985,16 +22118,32 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="64"/>
+      <c r="B20" s="59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="104">
+        <v>45371</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="63"/>
+      <c r="B21" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="71">
+        <v>173</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="70">
+        <v>45373</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
@@ -22295,10 +22444,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM340"/>
+  <dimension ref="A1:BM342"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -22367,43 +22516,43 @@
       <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="87"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="100"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="86"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="99"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -23165,23 +23314,23 @@
       <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="86"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="98"/>
+      <c r="F19" s="98"/>
+      <c r="G19" s="98"/>
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="99"/>
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24363,149 +24512,148 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45" s="75">
         <v>172</v>
       </c>
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="78">
         <v>200</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H45" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="I45" s="16" t="s">
+      <c r="I45" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="L45" s="5">
+      <c r="L45" s="79">
         <v>2611</v>
       </c>
-      <c r="M45" s="50" t="s">
+      <c r="M45" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="N45" s="22" t="s">
+      <c r="N45" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="O45" s="22" t="s">
+      <c r="O45" s="81" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="82" t="s">
+    <row r="46" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="82">
+        <v>174</v>
+      </c>
+      <c r="B46" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="84" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="85">
+        <v>200</v>
+      </c>
+      <c r="H46" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="J46" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="L46" s="86">
+        <v>2614</v>
+      </c>
+      <c r="M46" s="87" t="s">
+        <v>185</v>
+      </c>
+      <c r="N46" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="O46" s="83" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="101" t="s">
         <v>143</v>
       </c>
-      <c r="B46" s="83"/>
-      <c r="C46" s="83"/>
-      <c r="D46" s="83"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="83"/>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="83"/>
-      <c r="N46" s="83"/>
-      <c r="O46" s="87"/>
-      <c r="P46" s="13"/>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="84" t="s">
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="102"/>
+      <c r="F47" s="102"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="102"/>
+      <c r="J47" s="102"/>
+      <c r="K47" s="102"/>
+      <c r="L47" s="102"/>
+      <c r="M47" s="102"/>
+      <c r="N47" s="102"/>
+      <c r="O47" s="103"/>
+      <c r="P47" s="13"/>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="85"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="85"/>
-      <c r="K47" s="85"/>
-      <c r="L47" s="85"/>
-      <c r="M47" s="85"/>
-      <c r="N47" s="85"/>
-      <c r="O47" s="86"/>
-      <c r="P47" s="13"/>
-    </row>
-    <row r="48" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44">
+      <c r="B48" s="98"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="98"/>
+      <c r="N48" s="98"/>
+      <c r="O48" s="99"/>
+      <c r="P48" s="13"/>
+    </row>
+    <row r="49" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="44">
         <v>148</v>
-      </c>
-      <c r="B48" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="C48" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F48" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" s="44">
-        <v>403</v>
-      </c>
-      <c r="H48" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J48" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K48" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L48" s="44">
-        <v>1111</v>
-      </c>
-      <c r="M48" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="N48" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O48" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="P48" s="13"/>
-    </row>
-    <row r="49" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="44">
-        <v>146</v>
       </c>
       <c r="B49" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="D49" s="44" t="s">
         <v>36</v>
@@ -24532,76 +24680,76 @@
         <v>41</v>
       </c>
       <c r="L49" s="44">
-        <v>1016</v>
+        <v>1111</v>
       </c>
       <c r="M49" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N49" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O49" s="45" t="s">
-        <v>36</v>
+        <v>146</v>
+      </c>
+      <c r="N49" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="P49" s="13"/>
     </row>
-    <row r="50" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
-        <v>52</v>
+    <row r="50" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="44">
+        <v>146</v>
       </c>
       <c r="B50" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G50" s="16">
-        <v>401</v>
-      </c>
-      <c r="H50" s="35" t="s">
+      <c r="G50" s="44">
+        <v>403</v>
+      </c>
+      <c r="H50" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I50" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="L50" s="4">
-        <v>1012</v>
-      </c>
-      <c r="M50" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N50" s="23" t="s">
+      <c r="L50" s="44">
+        <v>1016</v>
+      </c>
+      <c r="M50" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N50" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O50" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="O50" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>45</v>
+      <c r="C51" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>36</v>
@@ -24628,28 +24776,28 @@
         <v>41</v>
       </c>
       <c r="L51" s="4">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N51" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O51" s="29" t="s">
+      <c r="O51" s="30" t="s">
         <v>36</v>
       </c>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B52" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>36</v>
@@ -24661,7 +24809,7 @@
         <v>37</v>
       </c>
       <c r="G52" s="16">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H52" s="35" t="s">
         <v>38</v>
@@ -24669,34 +24817,35 @@
       <c r="I52" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J52" s="16" t="s">
+      <c r="J52" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K52" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L52" s="16">
-        <v>1003</v>
-      </c>
-      <c r="M52" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="N52" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L52" s="4">
+        <v>1013</v>
+      </c>
+      <c r="M52" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N52" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O52" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P52" s="13"/>
+    </row>
+    <row r="53" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>36</v>
@@ -24708,7 +24857,7 @@
         <v>37</v>
       </c>
       <c r="G53" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H53" s="35" t="s">
         <v>38</v>
@@ -24720,13 +24869,13 @@
         <v>40</v>
       </c>
       <c r="K53" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L53" s="17">
-        <v>1004</v>
+        <v>47</v>
+      </c>
+      <c r="L53" s="16">
+        <v>1003</v>
       </c>
       <c r="M53" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N53" s="22" t="s">
         <v>147</v>
@@ -24735,15 +24884,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B54" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>53</v>
+      <c r="C54" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>36</v>
@@ -24755,7 +24904,7 @@
         <v>37</v>
       </c>
       <c r="G54" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H54" s="35" t="s">
         <v>38</v>
@@ -24763,94 +24912,45 @@
       <c r="I54" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="J54" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K54" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L54" s="5">
-        <v>1005</v>
-      </c>
-      <c r="M54" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="N54" s="23" t="s">
-        <v>42</v>
+      <c r="K54" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" s="17">
+        <v>1004</v>
+      </c>
+      <c r="M54" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="N54" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="O54" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
-      <c r="U54" s="14"/>
-      <c r="V54" s="14"/>
-      <c r="W54" s="14"/>
-      <c r="X54" s="14"/>
-      <c r="Y54" s="14"/>
-      <c r="Z54" s="14"/>
-      <c r="AA54" s="14"/>
-      <c r="AB54" s="14"/>
-      <c r="AC54" s="14"/>
-      <c r="AD54" s="14"/>
-      <c r="AE54" s="14"/>
-      <c r="AF54" s="14"/>
-      <c r="AG54" s="14"/>
-      <c r="AH54" s="14"/>
-      <c r="AI54" s="14"/>
-      <c r="AJ54" s="14"/>
-      <c r="AK54" s="14"/>
-      <c r="AL54" s="14"/>
-      <c r="AM54" s="14"/>
-      <c r="AN54" s="14"/>
-      <c r="AO54" s="14"/>
-      <c r="AP54" s="14"/>
-      <c r="AQ54" s="14"/>
-      <c r="AR54" s="14"/>
-      <c r="AS54" s="14"/>
-      <c r="AT54" s="14"/>
-      <c r="AU54" s="14"/>
-      <c r="AV54" s="14"/>
-      <c r="AW54" s="14"/>
-      <c r="AX54" s="14"/>
-      <c r="AY54" s="14"/>
-      <c r="AZ54" s="14"/>
-      <c r="BA54" s="14"/>
-      <c r="BB54" s="14"/>
-      <c r="BC54" s="14"/>
-      <c r="BD54" s="14"/>
-      <c r="BE54" s="14"/>
-      <c r="BF54" s="14"/>
-      <c r="BG54" s="14"/>
-      <c r="BH54" s="14"/>
-      <c r="BI54" s="14"/>
-      <c r="BJ54" s="14"/>
-      <c r="BK54" s="14"/>
-      <c r="BL54" s="14"/>
-      <c r="BM54" s="14"/>
-    </row>
-    <row r="55" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B55" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="54" t="s">
+      <c r="C55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E55" s="54" t="s">
+      <c r="E55" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F55" s="54" t="s">
+      <c r="F55" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="16">
         <v>403</v>
       </c>
       <c r="H55" s="35" t="s">
@@ -24859,45 +24959,94 @@
       <c r="I55" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J55" s="54" t="s">
+      <c r="J55" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L55" s="54">
-        <v>1015</v>
+        <v>47</v>
+      </c>
+      <c r="L55" s="5">
+        <v>1005</v>
       </c>
       <c r="M55" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="N55" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N55" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="O55" s="55" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O55" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="14"/>
+      <c r="X55" s="14"/>
+      <c r="Y55" s="14"/>
+      <c r="Z55" s="14"/>
+      <c r="AA55" s="14"/>
+      <c r="AB55" s="14"/>
+      <c r="AC55" s="14"/>
+      <c r="AD55" s="14"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="14"/>
+      <c r="AI55" s="14"/>
+      <c r="AJ55" s="14"/>
+      <c r="AK55" s="14"/>
+      <c r="AL55" s="14"/>
+      <c r="AM55" s="14"/>
+      <c r="AN55" s="14"/>
+      <c r="AO55" s="14"/>
+      <c r="AP55" s="14"/>
+      <c r="AQ55" s="14"/>
+      <c r="AR55" s="14"/>
+      <c r="AS55" s="14"/>
+      <c r="AT55" s="14"/>
+      <c r="AU55" s="14"/>
+      <c r="AV55" s="14"/>
+      <c r="AW55" s="14"/>
+      <c r="AX55" s="14"/>
+      <c r="AY55" s="14"/>
+      <c r="AZ55" s="14"/>
+      <c r="BA55" s="14"/>
+      <c r="BB55" s="14"/>
+      <c r="BC55" s="14"/>
+      <c r="BD55" s="14"/>
+      <c r="BE55" s="14"/>
+      <c r="BF55" s="14"/>
+      <c r="BG55" s="14"/>
+      <c r="BH55" s="14"/>
+      <c r="BI55" s="14"/>
+      <c r="BJ55" s="14"/>
+      <c r="BK55" s="14"/>
+      <c r="BL55" s="14"/>
+      <c r="BM55" s="14"/>
+    </row>
+    <row r="56" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="B56" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G56" s="16">
+      <c r="G56" s="4">
         <v>403</v>
       </c>
       <c r="H56" s="35" t="s">
@@ -24906,34 +25055,34 @@
       <c r="I56" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J56" s="16" t="s">
+      <c r="J56" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="K56" s="16" t="s">
+      <c r="K56" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L56" s="17">
-        <v>1006</v>
-      </c>
-      <c r="M56" s="23" t="s">
-        <v>57</v>
+      <c r="L56" s="54">
+        <v>1015</v>
+      </c>
+      <c r="M56" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="N56" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O56" s="22" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="O56" s="55" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>36</v>
@@ -24957,13 +25106,13 @@
         <v>40</v>
       </c>
       <c r="K57" s="16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L57" s="17">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M57" s="23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N57" s="22" t="s">
         <v>147</v>
@@ -24972,15 +25121,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>151</v>
+        <v>59</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>36</v>
@@ -25007,10 +25156,10 @@
         <v>47</v>
       </c>
       <c r="L58" s="17">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M58" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N58" s="22" t="s">
         <v>147</v>
@@ -25021,15 +25170,15 @@
     </row>
     <row r="59" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D59" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -25051,32 +25200,32 @@
         <v>40</v>
       </c>
       <c r="K59" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L59" s="16">
-        <v>1011</v>
+        <v>47</v>
+      </c>
+      <c r="L59" s="17">
+        <v>1008</v>
       </c>
       <c r="M59" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N59" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O59" s="22" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D60" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -25086,7 +25235,7 @@
         <v>37</v>
       </c>
       <c r="G60" s="16">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H60" s="35" t="s">
         <v>38</v>
@@ -25094,122 +25243,121 @@
       <c r="I60" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J60" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K60" s="4" t="s">
+      <c r="K60" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="L60" s="4">
+      <c r="L60" s="16">
+        <v>1011</v>
+      </c>
+      <c r="M60" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="N60" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O60" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>61</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="16">
+        <v>404</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I61" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L61" s="4">
         <v>2501</v>
       </c>
-      <c r="M60" s="22" t="s">
+      <c r="M61" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="N60" s="22" t="s">
+      <c r="N61" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="O60" s="22" t="s">
+      <c r="O61" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="82" t="s">
+    <row r="62" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="83"/>
-      <c r="C61" s="83"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="83"/>
-      <c r="F61" s="83"/>
-      <c r="G61" s="83"/>
-      <c r="H61" s="83"/>
-      <c r="I61" s="83"/>
-      <c r="J61" s="83"/>
-      <c r="K61" s="83"/>
-      <c r="L61" s="83"/>
-      <c r="M61" s="83"/>
-      <c r="N61" s="83"/>
-      <c r="O61" s="87"/>
-      <c r="P61" s="13"/>
-    </row>
-    <row r="62" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="84" t="s">
+      <c r="B62" s="96"/>
+      <c r="C62" s="96"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="96"/>
+      <c r="F62" s="96"/>
+      <c r="G62" s="96"/>
+      <c r="H62" s="96"/>
+      <c r="I62" s="96"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+      <c r="L62" s="96"/>
+      <c r="M62" s="96"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="100"/>
+      <c r="P62" s="13"/>
+    </row>
+    <row r="63" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="85"/>
-      <c r="C62" s="85"/>
-      <c r="D62" s="85"/>
-      <c r="E62" s="85"/>
-      <c r="F62" s="85"/>
-      <c r="G62" s="85"/>
-      <c r="H62" s="85"/>
-      <c r="I62" s="85"/>
-      <c r="J62" s="85"/>
-      <c r="K62" s="85"/>
-      <c r="L62" s="85"/>
-      <c r="M62" s="85"/>
-      <c r="N62" s="85"/>
-      <c r="O62" s="86"/>
-      <c r="P62" s="13"/>
-    </row>
-    <row r="63" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44">
+      <c r="B63" s="98"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="98"/>
+      <c r="F63" s="98"/>
+      <c r="G63" s="98"/>
+      <c r="H63" s="98"/>
+      <c r="I63" s="98"/>
+      <c r="J63" s="98"/>
+      <c r="K63" s="98"/>
+      <c r="L63" s="98"/>
+      <c r="M63" s="98"/>
+      <c r="N63" s="98"/>
+      <c r="O63" s="99"/>
+      <c r="P63" s="13"/>
+    </row>
+    <row r="64" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44">
         <v>148</v>
-      </c>
-      <c r="B63" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D63" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F63" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G63" s="44">
-        <v>403</v>
-      </c>
-      <c r="H63" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J63" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K63" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L63" s="44">
-        <v>1111</v>
-      </c>
-      <c r="M63" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="N63" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O63" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="P63" s="13"/>
-    </row>
-    <row r="64" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44">
-        <v>146</v>
       </c>
       <c r="B64" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
       <c r="D64" s="44" t="s">
         <v>36</v>
@@ -25236,76 +25384,76 @@
         <v>41</v>
       </c>
       <c r="L64" s="44">
-        <v>1016</v>
+        <v>1111</v>
       </c>
       <c r="M64" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N64" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O64" s="45" t="s">
-        <v>36</v>
+        <v>146</v>
+      </c>
+      <c r="N64" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O64" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="P64" s="13"/>
     </row>
-    <row r="65" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
-        <v>62</v>
+    <row r="65" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="44">
+        <v>146</v>
       </c>
       <c r="B65" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C65" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D65" s="4" t="s">
+      <c r="C65" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G65" s="16">
-        <v>401</v>
-      </c>
-      <c r="H65" s="35" t="s">
+      <c r="G65" s="44">
+        <v>403</v>
+      </c>
+      <c r="H65" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I65" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="J65" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K65" s="4" t="s">
+      <c r="K65" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="L65" s="4">
-        <v>1012</v>
-      </c>
-      <c r="M65" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N65" s="23" t="s">
+      <c r="L65" s="44">
+        <v>1016</v>
+      </c>
+      <c r="M65" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N65" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O65" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="O65" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="P65" s="13"/>
     </row>
-    <row r="66" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B66" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>36</v>
@@ -25332,28 +25480,28 @@
         <v>41</v>
       </c>
       <c r="L66" s="4">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M66" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N66" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O66" s="29" t="s">
+      <c r="O66" s="30" t="s">
         <v>36</v>
       </c>
       <c r="P66" s="13"/>
     </row>
-    <row r="67" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B67" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>36</v>
@@ -25365,7 +25513,7 @@
         <v>37</v>
       </c>
       <c r="G67" s="16">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H67" s="35" t="s">
         <v>38</v>
@@ -25373,34 +25521,35 @@
       <c r="I67" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J67" s="17" t="s">
+      <c r="J67" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K67" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L67" s="17">
-        <v>1003</v>
-      </c>
-      <c r="M67" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="N67" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O67" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K67" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L67" s="4">
+        <v>1013</v>
+      </c>
+      <c r="M67" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N67" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O67" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P67" s="13"/>
+    </row>
+    <row r="68" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>149</v>
+        <v>46</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>36</v>
@@ -25412,7 +25561,7 @@
         <v>37</v>
       </c>
       <c r="G68" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H68" s="35" t="s">
         <v>38</v>
@@ -25420,34 +25569,34 @@
       <c r="I68" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J68" s="16" t="s">
+      <c r="J68" s="17" t="s">
         <v>40</v>
       </c>
       <c r="K68" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L68" s="17">
-        <v>1004</v>
-      </c>
-      <c r="M68" s="22" t="s">
-        <v>52</v>
+        <v>1003</v>
+      </c>
+      <c r="M68" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="N68" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="O68" s="22" t="s">
+      <c r="O68" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B69" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>53</v>
+      <c r="C69" s="15" t="s">
+        <v>149</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>36</v>
@@ -25459,7 +25608,7 @@
         <v>37</v>
       </c>
       <c r="G69" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H69" s="35" t="s">
         <v>38</v>
@@ -25467,94 +25616,45 @@
       <c r="I69" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J69" s="4" t="s">
+      <c r="J69" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K69" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L69" s="5">
-        <v>1005</v>
+      <c r="K69" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L69" s="17">
+        <v>1004</v>
       </c>
       <c r="M69" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="N69" s="23" t="s">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c r="N69" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="O69" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Q69" s="14"/>
-      <c r="R69" s="14"/>
-      <c r="S69" s="14"/>
-      <c r="T69" s="14"/>
-      <c r="U69" s="14"/>
-      <c r="V69" s="14"/>
-      <c r="W69" s="14"/>
-      <c r="X69" s="14"/>
-      <c r="Y69" s="14"/>
-      <c r="Z69" s="14"/>
-      <c r="AA69" s="14"/>
-      <c r="AB69" s="14"/>
-      <c r="AC69" s="14"/>
-      <c r="AD69" s="14"/>
-      <c r="AE69" s="14"/>
-      <c r="AF69" s="14"/>
-      <c r="AG69" s="14"/>
-      <c r="AH69" s="14"/>
-      <c r="AI69" s="14"/>
-      <c r="AJ69" s="14"/>
-      <c r="AK69" s="14"/>
-      <c r="AL69" s="14"/>
-      <c r="AM69" s="14"/>
-      <c r="AN69" s="14"/>
-      <c r="AO69" s="14"/>
-      <c r="AP69" s="14"/>
-      <c r="AQ69" s="14"/>
-      <c r="AR69" s="14"/>
-      <c r="AS69" s="14"/>
-      <c r="AT69" s="14"/>
-      <c r="AU69" s="14"/>
-      <c r="AV69" s="14"/>
-      <c r="AW69" s="14"/>
-      <c r="AX69" s="14"/>
-      <c r="AY69" s="14"/>
-      <c r="AZ69" s="14"/>
-      <c r="BA69" s="14"/>
-      <c r="BB69" s="14"/>
-      <c r="BC69" s="14"/>
-      <c r="BD69" s="14"/>
-      <c r="BE69" s="14"/>
-      <c r="BF69" s="14"/>
-      <c r="BG69" s="14"/>
-      <c r="BH69" s="14"/>
-      <c r="BI69" s="14"/>
-      <c r="BJ69" s="14"/>
-      <c r="BK69" s="14"/>
-      <c r="BL69" s="14"/>
-      <c r="BM69" s="14"/>
-    </row>
-    <row r="70" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>118</v>
+        <v>77</v>
       </c>
       <c r="B70" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D70" s="54" t="s">
+      <c r="C70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E70" s="54" t="s">
+      <c r="E70" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F70" s="54" t="s">
+      <c r="F70" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G70" s="4">
+      <c r="G70" s="16">
         <v>403</v>
       </c>
       <c r="H70" s="35" t="s">
@@ -25563,45 +25663,94 @@
       <c r="I70" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J70" s="54" t="s">
+      <c r="J70" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K70" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L70" s="54">
-        <v>1015</v>
+        <v>47</v>
+      </c>
+      <c r="L70" s="5">
+        <v>1005</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="N70" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N70" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="O70" s="55" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O70" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14"/>
+      <c r="Z70" s="14"/>
+      <c r="AA70" s="14"/>
+      <c r="AB70" s="14"/>
+      <c r="AC70" s="14"/>
+      <c r="AD70" s="14"/>
+      <c r="AE70" s="14"/>
+      <c r="AF70" s="14"/>
+      <c r="AG70" s="14"/>
+      <c r="AH70" s="14"/>
+      <c r="AI70" s="14"/>
+      <c r="AJ70" s="14"/>
+      <c r="AK70" s="14"/>
+      <c r="AL70" s="14"/>
+      <c r="AM70" s="14"/>
+      <c r="AN70" s="14"/>
+      <c r="AO70" s="14"/>
+      <c r="AP70" s="14"/>
+      <c r="AQ70" s="14"/>
+      <c r="AR70" s="14"/>
+      <c r="AS70" s="14"/>
+      <c r="AT70" s="14"/>
+      <c r="AU70" s="14"/>
+      <c r="AV70" s="14"/>
+      <c r="AW70" s="14"/>
+      <c r="AX70" s="14"/>
+      <c r="AY70" s="14"/>
+      <c r="AZ70" s="14"/>
+      <c r="BA70" s="14"/>
+      <c r="BB70" s="14"/>
+      <c r="BC70" s="14"/>
+      <c r="BD70" s="14"/>
+      <c r="BE70" s="14"/>
+      <c r="BF70" s="14"/>
+      <c r="BG70" s="14"/>
+      <c r="BH70" s="14"/>
+      <c r="BI70" s="14"/>
+      <c r="BJ70" s="14"/>
+      <c r="BK70" s="14"/>
+      <c r="BL70" s="14"/>
+      <c r="BM70" s="14"/>
+    </row>
+    <row r="71" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="B71" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D71" s="4" t="s">
+      <c r="C71" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G71" s="16">
+      <c r="G71" s="4">
         <v>403</v>
       </c>
       <c r="H71" s="35" t="s">
@@ -25610,34 +25759,34 @@
       <c r="I71" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J71" s="16" t="s">
+      <c r="J71" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="K71" s="16" t="s">
+      <c r="K71" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L71" s="17">
-        <v>1006</v>
+      <c r="L71" s="54">
+        <v>1015</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N71" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O71" s="22" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="O71" s="55" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B72" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>36</v>
@@ -25661,13 +25810,13 @@
         <v>40</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L72" s="17">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M72" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N72" s="22" t="s">
         <v>147</v>
@@ -25678,13 +25827,13 @@
     </row>
     <row r="73" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>36</v>
@@ -25711,10 +25860,10 @@
         <v>47</v>
       </c>
       <c r="L73" s="17">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M73" s="22" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="N73" s="22" t="s">
         <v>147</v>
@@ -25725,15 +25874,15 @@
     </row>
     <row r="74" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B74" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D74" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E74" s="4" t="s">
@@ -25755,32 +25904,32 @@
         <v>40</v>
       </c>
       <c r="K74" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L74" s="16">
-        <v>1011</v>
-      </c>
-      <c r="M74" s="23" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="L74" s="17">
+        <v>1008</v>
+      </c>
+      <c r="M74" s="22" t="s">
+        <v>156</v>
       </c>
       <c r="N74" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O74" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B75" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D75" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E75" s="4" t="s">
@@ -25790,7 +25939,7 @@
         <v>37</v>
       </c>
       <c r="G75" s="16">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H75" s="35" t="s">
         <v>38</v>
@@ -25798,112 +25947,90 @@
       <c r="I75" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="J75" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K75" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L75" s="5">
-        <v>2506</v>
-      </c>
-      <c r="M75" s="22" t="s">
-        <v>158</v>
+      <c r="K75" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L75" s="16">
+        <v>1011</v>
+      </c>
+      <c r="M75" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="N75" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O75" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>71</v>
+      </c>
+      <c r="B76" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G76" s="16">
+        <v>404</v>
+      </c>
+      <c r="H76" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L76" s="5">
+        <v>2506</v>
+      </c>
+      <c r="M76" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="N76" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O76" s="22" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="82" t="s">
+    <row r="77" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="B76" s="83"/>
-      <c r="C76" s="83"/>
-      <c r="D76" s="83"/>
-      <c r="E76" s="83"/>
-      <c r="F76" s="83"/>
-      <c r="G76" s="83"/>
-      <c r="H76" s="83"/>
-      <c r="I76" s="83"/>
-      <c r="J76" s="83"/>
-      <c r="K76" s="83"/>
-      <c r="L76" s="83"/>
-      <c r="M76" s="83"/>
-      <c r="N76" s="83"/>
-      <c r="O76" s="83"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="13"/>
-      <c r="R76" s="13"/>
-      <c r="S76" s="13"/>
-      <c r="T76" s="13"/>
-      <c r="U76" s="13"/>
-      <c r="V76" s="13"/>
-      <c r="W76" s="13"/>
-      <c r="X76" s="13"/>
-      <c r="Y76" s="13"/>
-      <c r="Z76" s="13"/>
-      <c r="AA76" s="13"/>
-      <c r="AB76" s="13"/>
-      <c r="AC76" s="13"/>
-      <c r="AD76" s="13"/>
-      <c r="AE76" s="13"/>
-      <c r="AF76" s="13"/>
-      <c r="AG76" s="13"/>
-      <c r="AH76" s="13"/>
-      <c r="AI76" s="13"/>
-      <c r="AJ76" s="13"/>
-      <c r="AK76" s="13"/>
-      <c r="AL76" s="13"/>
-      <c r="AM76" s="13"/>
-      <c r="AN76" s="13"/>
-      <c r="AO76" s="13"/>
-      <c r="AP76" s="13"/>
-      <c r="AQ76" s="13"/>
-      <c r="AR76" s="13"/>
-      <c r="AS76" s="13"/>
-      <c r="AT76" s="13"/>
-      <c r="AU76" s="13"/>
-      <c r="AV76" s="13"/>
-      <c r="AW76" s="13"/>
-      <c r="AX76" s="13"/>
-      <c r="AY76" s="13"/>
-      <c r="AZ76" s="13"/>
-      <c r="BA76" s="13"/>
-      <c r="BB76" s="13"/>
-      <c r="BC76" s="13"/>
-      <c r="BD76" s="13"/>
-      <c r="BE76" s="13"/>
-      <c r="BF76" s="13"/>
-      <c r="BG76" s="13"/>
-      <c r="BH76" s="13"/>
-      <c r="BI76" s="13"/>
-      <c r="BJ76" s="13"/>
-      <c r="BK76" s="13"/>
-      <c r="BL76" s="13"/>
-      <c r="BM76" s="13"/>
-    </row>
-    <row r="77" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="B77" s="85"/>
-      <c r="C77" s="85"/>
-      <c r="D77" s="85"/>
-      <c r="E77" s="85"/>
-      <c r="F77" s="85"/>
-      <c r="G77" s="85"/>
-      <c r="H77" s="85"/>
-      <c r="I77" s="85"/>
-      <c r="J77" s="85"/>
-      <c r="K77" s="85"/>
-      <c r="L77" s="85"/>
-      <c r="M77" s="85"/>
-      <c r="N77" s="85"/>
-      <c r="O77" s="85"/>
+      <c r="B77" s="96"/>
+      <c r="C77" s="96"/>
+      <c r="D77" s="96"/>
+      <c r="E77" s="96"/>
+      <c r="F77" s="96"/>
+      <c r="G77" s="96"/>
+      <c r="H77" s="96"/>
+      <c r="I77" s="96"/>
+      <c r="J77" s="96"/>
+      <c r="K77" s="96"/>
+      <c r="L77" s="96"/>
+      <c r="M77" s="96"/>
+      <c r="N77" s="96"/>
+      <c r="O77" s="96"/>
       <c r="P77" s="13"/>
       <c r="Q77" s="13"/>
       <c r="R77" s="13"/>
@@ -25955,52 +26082,24 @@
       <c r="BL77" s="13"/>
       <c r="BM77" s="13"/>
     </row>
-    <row r="78" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="44">
-        <v>146</v>
-      </c>
-      <c r="B78" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="C78" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D78" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E78" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F78" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G78" s="44">
-        <v>403</v>
-      </c>
-      <c r="H78" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I78" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J78" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K78" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L78" s="44">
-        <v>1016</v>
-      </c>
-      <c r="M78" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N78" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O78" s="45" t="s">
-        <v>36</v>
-      </c>
+    <row r="78" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" s="98"/>
+      <c r="C78" s="98"/>
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="98"/>
+      <c r="H78" s="98"/>
+      <c r="I78" s="98"/>
+      <c r="J78" s="98"/>
+      <c r="K78" s="98"/>
+      <c r="L78" s="98"/>
+      <c r="M78" s="98"/>
+      <c r="N78" s="98"/>
+      <c r="O78" s="98"/>
       <c r="P78" s="13"/>
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
@@ -26052,50 +26151,50 @@
       <c r="BL78" s="13"/>
       <c r="BM78" s="13"/>
     </row>
-    <row r="79" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
-        <v>72</v>
+    <row r="79" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="44">
+        <v>146</v>
       </c>
       <c r="B79" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C79" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D79" s="4" t="s">
+      <c r="C79" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E79" s="4" t="s">
+      <c r="E79" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F79" s="4" t="s">
+      <c r="F79" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G79" s="16">
-        <v>401</v>
-      </c>
-      <c r="H79" s="35" t="s">
+      <c r="G79" s="44">
+        <v>403</v>
+      </c>
+      <c r="H79" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I79" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J79" s="4" t="s">
+      <c r="J79" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K79" s="4" t="s">
+      <c r="K79" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="L79" s="4">
-        <v>1012</v>
-      </c>
-      <c r="M79" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N79" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O79" s="30" t="s">
+      <c r="L79" s="44">
+        <v>1016</v>
+      </c>
+      <c r="M79" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N79" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O79" s="45" t="s">
         <v>36</v>
       </c>
       <c r="P79" s="13"/>
@@ -26149,15 +26248,15 @@
       <c r="BL79" s="13"/>
       <c r="BM79" s="13"/>
     </row>
-    <row r="80" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>36</v>
@@ -26184,15 +26283,15 @@
         <v>41</v>
       </c>
       <c r="L80" s="4">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M80" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N80" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O80" s="29" t="s">
+      <c r="O80" s="30" t="s">
         <v>36</v>
       </c>
       <c r="P80" s="13"/>
@@ -26246,15 +26345,15 @@
       <c r="BL80" s="13"/>
       <c r="BM80" s="13"/>
     </row>
-    <row r="81" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B81" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>36</v>
@@ -26266,7 +26365,7 @@
         <v>37</v>
       </c>
       <c r="G81" s="16">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H81" s="35" t="s">
         <v>38</v>
@@ -26278,79 +26377,80 @@
         <v>40</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L81" s="5">
-        <v>1003</v>
-      </c>
-      <c r="M81" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="N81" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="O81" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q81" s="14"/>
-      <c r="R81" s="14"/>
-      <c r="S81" s="14"/>
-      <c r="T81" s="14"/>
-      <c r="U81" s="14"/>
-      <c r="V81" s="14"/>
-      <c r="W81" s="14"/>
-      <c r="X81" s="14"/>
-      <c r="Y81" s="14"/>
-      <c r="Z81" s="14"/>
-      <c r="AA81" s="14"/>
-      <c r="AB81" s="14"/>
-      <c r="AC81" s="14"/>
-      <c r="AD81" s="14"/>
-      <c r="AE81" s="14"/>
-      <c r="AF81" s="14"/>
-      <c r="AG81" s="14"/>
-      <c r="AH81" s="14"/>
-      <c r="AI81" s="14"/>
-      <c r="AJ81" s="14"/>
-      <c r="AK81" s="14"/>
-      <c r="AL81" s="14"/>
-      <c r="AM81" s="14"/>
-      <c r="AN81" s="14"/>
-      <c r="AO81" s="14"/>
-      <c r="AP81" s="14"/>
-      <c r="AQ81" s="14"/>
-      <c r="AR81" s="14"/>
-      <c r="AS81" s="14"/>
-      <c r="AT81" s="14"/>
-      <c r="AU81" s="14"/>
-      <c r="AV81" s="14"/>
-      <c r="AW81" s="14"/>
-      <c r="AX81" s="14"/>
-      <c r="AY81" s="14"/>
-      <c r="AZ81" s="14"/>
-      <c r="BA81" s="14"/>
-      <c r="BB81" s="14"/>
-      <c r="BC81" s="14"/>
-      <c r="BD81" s="14"/>
-      <c r="BE81" s="14"/>
-      <c r="BF81" s="14"/>
-      <c r="BG81" s="14"/>
-      <c r="BH81" s="14"/>
-      <c r="BI81" s="14"/>
-      <c r="BJ81" s="14"/>
-      <c r="BK81" s="14"/>
-      <c r="BL81" s="14"/>
-      <c r="BM81" s="14"/>
-    </row>
-    <row r="82" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="L81" s="4">
+        <v>1013</v>
+      </c>
+      <c r="M81" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N81" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O81" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P81" s="13"/>
+      <c r="Q81" s="13"/>
+      <c r="R81" s="13"/>
+      <c r="S81" s="13"/>
+      <c r="T81" s="13"/>
+      <c r="U81" s="13"/>
+      <c r="V81" s="13"/>
+      <c r="W81" s="13"/>
+      <c r="X81" s="13"/>
+      <c r="Y81" s="13"/>
+      <c r="Z81" s="13"/>
+      <c r="AA81" s="13"/>
+      <c r="AB81" s="13"/>
+      <c r="AC81" s="13"/>
+      <c r="AD81" s="13"/>
+      <c r="AE81" s="13"/>
+      <c r="AF81" s="13"/>
+      <c r="AG81" s="13"/>
+      <c r="AH81" s="13"/>
+      <c r="AI81" s="13"/>
+      <c r="AJ81" s="13"/>
+      <c r="AK81" s="13"/>
+      <c r="AL81" s="13"/>
+      <c r="AM81" s="13"/>
+      <c r="AN81" s="13"/>
+      <c r="AO81" s="13"/>
+      <c r="AP81" s="13"/>
+      <c r="AQ81" s="13"/>
+      <c r="AR81" s="13"/>
+      <c r="AS81" s="13"/>
+      <c r="AT81" s="13"/>
+      <c r="AU81" s="13"/>
+      <c r="AV81" s="13"/>
+      <c r="AW81" s="13"/>
+      <c r="AX81" s="13"/>
+      <c r="AY81" s="13"/>
+      <c r="AZ81" s="13"/>
+      <c r="BA81" s="13"/>
+      <c r="BB81" s="13"/>
+      <c r="BC81" s="13"/>
+      <c r="BD81" s="13"/>
+      <c r="BE81" s="13"/>
+      <c r="BF81" s="13"/>
+      <c r="BG81" s="13"/>
+      <c r="BH81" s="13"/>
+      <c r="BI81" s="13"/>
+      <c r="BJ81" s="13"/>
+      <c r="BK81" s="13"/>
+      <c r="BL81" s="13"/>
+      <c r="BM81" s="13"/>
+    </row>
+    <row r="82" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B82" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C82" s="3" t="s">
-        <v>50</v>
+      <c r="C82" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>36</v>
@@ -26362,7 +26462,7 @@
         <v>37</v>
       </c>
       <c r="G82" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H82" s="35" t="s">
         <v>38</v>
@@ -26374,13 +26474,13 @@
         <v>40</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L82" s="5">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M82" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N82" s="22" t="s">
         <v>162</v>
@@ -26438,15 +26538,15 @@
       <c r="BL82" s="14"/>
       <c r="BM82" s="14"/>
     </row>
-    <row r="83" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B83" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>36</v>
@@ -26458,7 +26558,7 @@
         <v>37</v>
       </c>
       <c r="G83" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H83" s="35" t="s">
         <v>38</v>
@@ -26470,13 +26570,13 @@
         <v>40</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L83" s="5">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="M83" s="22" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="N83" s="22" t="s">
         <v>162</v>
@@ -26534,26 +26634,26 @@
       <c r="BL83" s="14"/>
       <c r="BM83" s="14"/>
     </row>
-    <row r="84" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B84" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C84" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D84" s="54" t="s">
+      <c r="C84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E84" s="54" t="s">
+      <c r="E84" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F84" s="54" t="s">
+      <c r="F84" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G84" s="4">
+      <c r="G84" s="16">
         <v>403</v>
       </c>
       <c r="H84" s="35" t="s">
@@ -26562,23 +26662,23 @@
       <c r="I84" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J84" s="54" t="s">
+      <c r="J84" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L84" s="54">
-        <v>1015</v>
+        <v>47</v>
+      </c>
+      <c r="L84" s="5">
+        <v>1005</v>
       </c>
       <c r="M84" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N84" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O84" s="55" t="s">
-        <v>36</v>
+        <v>162</v>
+      </c>
+      <c r="O84" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="Q84" s="14"/>
       <c r="R84" s="14"/>
@@ -26630,26 +26730,26 @@
       <c r="BL84" s="14"/>
       <c r="BM84" s="14"/>
     </row>
-    <row r="85" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="B85" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="16">
+      <c r="G85" s="4">
         <v>403</v>
       </c>
       <c r="H85" s="35" t="s">
@@ -26658,23 +26758,23 @@
       <c r="I85" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="J85" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L85" s="5">
-        <v>1006</v>
+      <c r="L85" s="54">
+        <v>1015</v>
       </c>
       <c r="M85" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N85" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="O85" s="22" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="O85" s="55" t="s">
+        <v>36</v>
       </c>
       <c r="Q85" s="14"/>
       <c r="R85" s="14"/>
@@ -26728,13 +26828,13 @@
     </row>
     <row r="86" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B86" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>36</v>
@@ -26758,13 +26858,13 @@
         <v>40</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L86" s="5">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M86" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N86" s="22" t="s">
         <v>162</v>
@@ -26822,15 +26922,15 @@
       <c r="BL86" s="14"/>
       <c r="BM86" s="14"/>
     </row>
-    <row r="87" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B87" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>36</v>
@@ -26857,10 +26957,10 @@
         <v>47</v>
       </c>
       <c r="L87" s="5">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M87" s="22" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="N87" s="22" t="s">
         <v>162</v>
@@ -26920,13 +27020,13 @@
     </row>
     <row r="88" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>164</v>
+        <v>61</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>36</v>
@@ -26950,19 +27050,19 @@
         <v>40</v>
       </c>
       <c r="K88" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L88" s="5">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="M88" s="22" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
       <c r="N88" s="22" t="s">
         <v>162</v>
       </c>
       <c r="O88" s="22" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="Q88" s="14"/>
       <c r="R88" s="14"/>
@@ -27014,15 +27114,15 @@
       <c r="BL88" s="14"/>
       <c r="BM88" s="14"/>
     </row>
-    <row r="89" spans="1:65" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="18">
-        <v>169</v>
+    <row r="89" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>81</v>
       </c>
       <c r="B89" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C89" s="51" t="s">
-        <v>165</v>
+      <c r="C89" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>36</v>
@@ -27034,7 +27134,7 @@
         <v>37</v>
       </c>
       <c r="G89" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H89" s="35" t="s">
         <v>38</v>
@@ -27046,91 +27146,90 @@
         <v>40</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L89" s="18">
-        <v>3101</v>
-      </c>
-      <c r="M89" s="40" t="s">
-        <v>166</v>
+        <v>41</v>
+      </c>
+      <c r="L89" s="5">
+        <v>1011</v>
+      </c>
+      <c r="M89" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="N89" s="22" t="s">
         <v>162</v>
       </c>
       <c r="O89" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
-      <c r="S89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="13"/>
-      <c r="W89" s="13"/>
-      <c r="X89" s="13"/>
-      <c r="Y89" s="13"/>
-      <c r="Z89" s="13"/>
-      <c r="AA89" s="13"/>
-      <c r="AB89" s="13"/>
-      <c r="AC89" s="13"/>
-      <c r="AD89" s="13"/>
-      <c r="AE89" s="13"/>
-      <c r="AF89" s="13"/>
-      <c r="AG89" s="13"/>
-      <c r="AH89" s="13"/>
-      <c r="AI89" s="13"/>
-      <c r="AJ89" s="13"/>
-      <c r="AK89" s="13"/>
-      <c r="AL89" s="13"/>
-      <c r="AM89" s="13"/>
-      <c r="AN89" s="13"/>
-      <c r="AO89" s="13"/>
-      <c r="AP89" s="13"/>
-      <c r="AQ89" s="13"/>
-      <c r="AR89" s="13"/>
-      <c r="AS89" s="13"/>
-      <c r="AT89" s="13"/>
-      <c r="AU89" s="13"/>
-      <c r="AV89" s="13"/>
-      <c r="AW89" s="13"/>
-      <c r="AX89" s="13"/>
-      <c r="AY89" s="13"/>
-      <c r="AZ89" s="13"/>
-      <c r="BA89" s="13"/>
-      <c r="BB89" s="13"/>
-      <c r="BC89" s="13"/>
-      <c r="BD89" s="13"/>
-      <c r="BE89" s="13"/>
-      <c r="BF89" s="13"/>
-      <c r="BG89" s="13"/>
-      <c r="BH89" s="13"/>
-      <c r="BI89" s="13"/>
-      <c r="BJ89" s="13"/>
-      <c r="BK89" s="13"/>
-      <c r="BL89" s="13"/>
-      <c r="BM89" s="13"/>
-    </row>
-    <row r="90" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="35">
-        <v>156</v>
+        <v>36</v>
+      </c>
+      <c r="Q89" s="14"/>
+      <c r="R89" s="14"/>
+      <c r="S89" s="14"/>
+      <c r="T89" s="14"/>
+      <c r="U89" s="14"/>
+      <c r="V89" s="14"/>
+      <c r="W89" s="14"/>
+      <c r="X89" s="14"/>
+      <c r="Y89" s="14"/>
+      <c r="Z89" s="14"/>
+      <c r="AA89" s="14"/>
+      <c r="AB89" s="14"/>
+      <c r="AC89" s="14"/>
+      <c r="AD89" s="14"/>
+      <c r="AE89" s="14"/>
+      <c r="AF89" s="14"/>
+      <c r="AG89" s="14"/>
+      <c r="AH89" s="14"/>
+      <c r="AI89" s="14"/>
+      <c r="AJ89" s="14"/>
+      <c r="AK89" s="14"/>
+      <c r="AL89" s="14"/>
+      <c r="AM89" s="14"/>
+      <c r="AN89" s="14"/>
+      <c r="AO89" s="14"/>
+      <c r="AP89" s="14"/>
+      <c r="AQ89" s="14"/>
+      <c r="AR89" s="14"/>
+      <c r="AS89" s="14"/>
+      <c r="AT89" s="14"/>
+      <c r="AU89" s="14"/>
+      <c r="AV89" s="14"/>
+      <c r="AW89" s="14"/>
+      <c r="AX89" s="14"/>
+      <c r="AY89" s="14"/>
+      <c r="AZ89" s="14"/>
+      <c r="BA89" s="14"/>
+      <c r="BB89" s="14"/>
+      <c r="BC89" s="14"/>
+      <c r="BD89" s="14"/>
+      <c r="BE89" s="14"/>
+      <c r="BF89" s="14"/>
+      <c r="BG89" s="14"/>
+      <c r="BH89" s="14"/>
+      <c r="BI89" s="14"/>
+      <c r="BJ89" s="14"/>
+      <c r="BK89" s="14"/>
+      <c r="BL89" s="14"/>
+      <c r="BM89" s="14"/>
+    </row>
+    <row r="90" spans="1:65" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="18">
+        <v>169</v>
       </c>
       <c r="B90" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C90" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="D90" s="35" t="s">
+      <c r="C90" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E90" s="35" t="s">
+      <c r="E90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F90" s="35" t="s">
+      <c r="F90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G90" s="35">
+      <c r="G90" s="16">
         <v>400</v>
       </c>
       <c r="H90" s="35" t="s">
@@ -27139,23 +27238,23 @@
       <c r="I90" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J90" s="35" t="s">
+      <c r="J90" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K90" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="L90" s="35">
-        <v>3014</v>
-      </c>
-      <c r="M90" s="47" t="s">
-        <v>169</v>
+      <c r="K90" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L90" s="18">
+        <v>3101</v>
+      </c>
+      <c r="M90" s="40" t="s">
+        <v>166</v>
       </c>
       <c r="N90" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="O90" s="58" t="s">
-        <v>170</v>
+      <c r="O90" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="P90" s="13"/>
       <c r="Q90" s="13"/>
@@ -27208,294 +27307,344 @@
       <c r="BL90" s="13"/>
       <c r="BM90" s="13"/>
     </row>
-    <row r="91" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
-        <v>168</v>
+    <row r="91" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="35">
+        <v>156</v>
       </c>
       <c r="B91" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D91" s="4">
-        <v>9</v>
-      </c>
-      <c r="E91" s="16" t="s">
+      <c r="C91" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D91" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="16" t="s">
+      <c r="F91" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G91" s="16">
-        <v>200</v>
-      </c>
-      <c r="H91" s="16" t="s">
-        <v>80</v>
+      <c r="G91" s="35">
+        <v>400</v>
+      </c>
+      <c r="H91" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="I91" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="J91" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K91" s="4" t="s">
+      <c r="K91" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="L91" s="4">
-        <v>1010</v>
-      </c>
-      <c r="M91" s="22" t="s">
-        <v>99</v>
+      <c r="L91" s="35">
+        <v>3014</v>
+      </c>
+      <c r="M91" s="47" t="s">
+        <v>169</v>
       </c>
       <c r="N91" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="O91" s="22" t="s">
+      <c r="O91" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="P91" s="13"/>
+      <c r="Q91" s="13"/>
+      <c r="R91" s="13"/>
+      <c r="S91" s="13"/>
+      <c r="T91" s="13"/>
+      <c r="U91" s="13"/>
+      <c r="V91" s="13"/>
+      <c r="W91" s="13"/>
+      <c r="X91" s="13"/>
+      <c r="Y91" s="13"/>
+      <c r="Z91" s="13"/>
+      <c r="AA91" s="13"/>
+      <c r="AB91" s="13"/>
+      <c r="AC91" s="13"/>
+      <c r="AD91" s="13"/>
+      <c r="AE91" s="13"/>
+      <c r="AF91" s="13"/>
+      <c r="AG91" s="13"/>
+      <c r="AH91" s="13"/>
+      <c r="AI91" s="13"/>
+      <c r="AJ91" s="13"/>
+      <c r="AK91" s="13"/>
+      <c r="AL91" s="13"/>
+      <c r="AM91" s="13"/>
+      <c r="AN91" s="13"/>
+      <c r="AO91" s="13"/>
+      <c r="AP91" s="13"/>
+      <c r="AQ91" s="13"/>
+      <c r="AR91" s="13"/>
+      <c r="AS91" s="13"/>
+      <c r="AT91" s="13"/>
+      <c r="AU91" s="13"/>
+      <c r="AV91" s="13"/>
+      <c r="AW91" s="13"/>
+      <c r="AX91" s="13"/>
+      <c r="AY91" s="13"/>
+      <c r="AZ91" s="13"/>
+      <c r="BA91" s="13"/>
+      <c r="BB91" s="13"/>
+      <c r="BC91" s="13"/>
+      <c r="BD91" s="13"/>
+      <c r="BE91" s="13"/>
+      <c r="BF91" s="13"/>
+      <c r="BG91" s="13"/>
+      <c r="BH91" s="13"/>
+      <c r="BI91" s="13"/>
+      <c r="BJ91" s="13"/>
+      <c r="BK91" s="13"/>
+      <c r="BL91" s="13"/>
+      <c r="BM91" s="13"/>
+    </row>
+    <row r="92" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>168</v>
+      </c>
+      <c r="B92" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D92" s="4">
+        <v>9</v>
+      </c>
+      <c r="E92" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F92" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G92" s="16">
+        <v>200</v>
+      </c>
+      <c r="H92" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L92" s="4">
+        <v>1010</v>
+      </c>
+      <c r="M92" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="N92" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="O92" s="22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="82" t="s">
+    <row r="93" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>175</v>
+      </c>
+      <c r="B93" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D93" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F93" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G93" s="16">
+        <v>200</v>
+      </c>
+      <c r="H93" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I93" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L93" s="4">
+        <v>3015</v>
+      </c>
+      <c r="M93" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="N93" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="O93" s="22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="95" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="83"/>
-      <c r="C92" s="83"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="83"/>
-      <c r="F92" s="83"/>
-      <c r="G92" s="83"/>
-      <c r="H92" s="83"/>
-      <c r="I92" s="83"/>
-      <c r="J92" s="83"/>
-      <c r="K92" s="83"/>
-      <c r="L92" s="83"/>
-      <c r="M92" s="83"/>
-      <c r="N92" s="83"/>
-      <c r="O92" s="83"/>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="13"/>
-      <c r="R92" s="13"/>
-      <c r="S92" s="13"/>
-      <c r="T92" s="13"/>
-      <c r="U92" s="13"/>
-      <c r="V92" s="13"/>
-      <c r="W92" s="13"/>
-      <c r="X92" s="13"/>
-      <c r="Y92" s="13"/>
-      <c r="Z92" s="13"/>
-      <c r="AA92" s="13"/>
-      <c r="AB92" s="13"/>
-      <c r="AC92" s="13"/>
-      <c r="AD92" s="13"/>
-      <c r="AE92" s="13"/>
-      <c r="AF92" s="13"/>
-      <c r="AG92" s="13"/>
-      <c r="AH92" s="13"/>
-      <c r="AI92" s="13"/>
-      <c r="AJ92" s="13"/>
-      <c r="AK92" s="13"/>
-      <c r="AL92" s="13"/>
-      <c r="AM92" s="13"/>
-      <c r="AN92" s="13"/>
-      <c r="AO92" s="13"/>
-      <c r="AP92" s="13"/>
-      <c r="AQ92" s="13"/>
-      <c r="AR92" s="13"/>
-      <c r="AS92" s="13"/>
-      <c r="AT92" s="13"/>
-      <c r="AU92" s="13"/>
-      <c r="AV92" s="13"/>
-      <c r="AW92" s="13"/>
-      <c r="AX92" s="13"/>
-      <c r="AY92" s="13"/>
-      <c r="AZ92" s="13"/>
-      <c r="BA92" s="13"/>
-      <c r="BB92" s="13"/>
-      <c r="BC92" s="13"/>
-      <c r="BD92" s="13"/>
-      <c r="BE92" s="13"/>
-      <c r="BF92" s="13"/>
-      <c r="BG92" s="13"/>
-      <c r="BH92" s="13"/>
-      <c r="BI92" s="13"/>
-      <c r="BJ92" s="13"/>
-      <c r="BK92" s="13"/>
-      <c r="BL92" s="13"/>
-      <c r="BM92" s="13"/>
-    </row>
-    <row r="93" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="84" t="s">
+      <c r="B94" s="96"/>
+      <c r="C94" s="96"/>
+      <c r="D94" s="96"/>
+      <c r="E94" s="96"/>
+      <c r="F94" s="96"/>
+      <c r="G94" s="96"/>
+      <c r="H94" s="96"/>
+      <c r="I94" s="96"/>
+      <c r="J94" s="96"/>
+      <c r="K94" s="96"/>
+      <c r="L94" s="96"/>
+      <c r="M94" s="96"/>
+      <c r="N94" s="96"/>
+      <c r="O94" s="96"/>
+      <c r="P94" s="13"/>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="13"/>
+      <c r="V94" s="13"/>
+      <c r="W94" s="13"/>
+      <c r="X94" s="13"/>
+      <c r="Y94" s="13"/>
+      <c r="Z94" s="13"/>
+      <c r="AA94" s="13"/>
+      <c r="AB94" s="13"/>
+      <c r="AC94" s="13"/>
+      <c r="AD94" s="13"/>
+      <c r="AE94" s="13"/>
+      <c r="AF94" s="13"/>
+      <c r="AG94" s="13"/>
+      <c r="AH94" s="13"/>
+      <c r="AI94" s="13"/>
+      <c r="AJ94" s="13"/>
+      <c r="AK94" s="13"/>
+      <c r="AL94" s="13"/>
+      <c r="AM94" s="13"/>
+      <c r="AN94" s="13"/>
+      <c r="AO94" s="13"/>
+      <c r="AP94" s="13"/>
+      <c r="AQ94" s="13"/>
+      <c r="AR94" s="13"/>
+      <c r="AS94" s="13"/>
+      <c r="AT94" s="13"/>
+      <c r="AU94" s="13"/>
+      <c r="AV94" s="13"/>
+      <c r="AW94" s="13"/>
+      <c r="AX94" s="13"/>
+      <c r="AY94" s="13"/>
+      <c r="AZ94" s="13"/>
+      <c r="BA94" s="13"/>
+      <c r="BB94" s="13"/>
+      <c r="BC94" s="13"/>
+      <c r="BD94" s="13"/>
+      <c r="BE94" s="13"/>
+      <c r="BF94" s="13"/>
+      <c r="BG94" s="13"/>
+      <c r="BH94" s="13"/>
+      <c r="BI94" s="13"/>
+      <c r="BJ94" s="13"/>
+      <c r="BK94" s="13"/>
+      <c r="BL94" s="13"/>
+      <c r="BM94" s="13"/>
+    </row>
+    <row r="95" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="85"/>
-      <c r="C93" s="85"/>
-      <c r="D93" s="85"/>
-      <c r="E93" s="85"/>
-      <c r="F93" s="85"/>
-      <c r="G93" s="85"/>
-      <c r="H93" s="85"/>
-      <c r="I93" s="85"/>
-      <c r="J93" s="85"/>
-      <c r="K93" s="85"/>
-      <c r="L93" s="85"/>
-      <c r="M93" s="85"/>
-      <c r="N93" s="85"/>
-      <c r="O93" s="85"/>
-    </row>
-    <row r="94" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A94" s="44">
+      <c r="B95" s="98"/>
+      <c r="C95" s="98"/>
+      <c r="D95" s="98"/>
+      <c r="E95" s="98"/>
+      <c r="F95" s="98"/>
+      <c r="G95" s="98"/>
+      <c r="H95" s="98"/>
+      <c r="I95" s="98"/>
+      <c r="J95" s="98"/>
+      <c r="K95" s="98"/>
+      <c r="L95" s="98"/>
+      <c r="M95" s="98"/>
+      <c r="N95" s="98"/>
+      <c r="O95" s="98"/>
+    </row>
+    <row r="96" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A96" s="44">
         <v>146</v>
-      </c>
-      <c r="B94" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C94" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D94" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="F94" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="G94" s="44">
-        <v>403</v>
-      </c>
-      <c r="H94" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="I94" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J94" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K94" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L94" s="4">
-        <v>1016</v>
-      </c>
-      <c r="M94" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N94" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O94" s="45" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="95" spans="1:65" ht="63" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
-        <v>102</v>
-      </c>
-      <c r="B95" s="57" t="s">
-        <v>172</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G95" s="16">
-        <v>401</v>
-      </c>
-      <c r="H95" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="I95" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K95" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L95" s="4">
-        <v>1012</v>
-      </c>
-      <c r="M95" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N95" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O95" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="96" spans="1:65" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>103</v>
       </c>
       <c r="B96" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C96" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D96" s="4" t="s">
+      <c r="C96" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="E96" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="F96" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G96" s="16">
-        <v>401</v>
-      </c>
-      <c r="H96" s="35" t="s">
+      <c r="G96" s="44">
+        <v>403</v>
+      </c>
+      <c r="H96" s="44" t="s">
         <v>38</v>
       </c>
       <c r="I96" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J96" s="4" t="s">
+      <c r="J96" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K96" s="4" t="s">
+      <c r="K96" s="44" t="s">
         <v>41</v>
       </c>
       <c r="L96" s="4">
-        <v>1013</v>
-      </c>
-      <c r="M96" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N96" s="23" t="s">
+        <v>1016</v>
+      </c>
+      <c r="M96" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N96" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O96" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="O96" s="29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B97" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D97" s="4">
-        <v>301</v>
+        <v>43</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>37</v>
@@ -27504,7 +27653,7 @@
         <v>37</v>
       </c>
       <c r="G97" s="16">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H97" s="35" t="s">
         <v>38</v>
@@ -27516,33 +27665,33 @@
         <v>40</v>
       </c>
       <c r="K97" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L97" s="5">
-        <v>1003</v>
-      </c>
-      <c r="M97" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="N97" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O97" s="22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="L97" s="4">
+        <v>1012</v>
+      </c>
+      <c r="M97" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N97" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O97" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B98" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D98" s="4">
-        <v>301</v>
+      <c r="C98" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>37</v>
@@ -27551,7 +27700,7 @@
         <v>37</v>
       </c>
       <c r="G98" s="16">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H98" s="35" t="s">
         <v>38</v>
@@ -27563,33 +27712,33 @@
         <v>40</v>
       </c>
       <c r="K98" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L98" s="5">
-        <v>1004</v>
-      </c>
-      <c r="M98" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="N98" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O98" s="22" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="L98" s="4">
+        <v>1013</v>
+      </c>
+      <c r="M98" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N98" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O98" s="29" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B99" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>36</v>
+      <c r="C99" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D99" s="4">
+        <v>301</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>37</v>
@@ -27610,42 +27759,42 @@
         <v>40</v>
       </c>
       <c r="K99" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L99" s="5">
-        <v>1015</v>
+        <v>1003</v>
       </c>
       <c r="M99" s="22" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="N99" s="22" t="s">
         <v>42</v>
       </c>
       <c r="O99" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C100" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D100" s="54">
-        <v>302</v>
-      </c>
-      <c r="E100" s="54" t="s">
+      <c r="C100" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="4">
+        <v>301</v>
+      </c>
+      <c r="E100" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F100" s="54" t="s">
+      <c r="F100" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G100" s="4">
-        <v>403</v>
+      <c r="G100" s="16">
+        <v>400</v>
       </c>
       <c r="H100" s="35" t="s">
         <v>38</v>
@@ -27653,37 +27802,37 @@
       <c r="I100" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J100" s="54" t="s">
+      <c r="J100" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K100" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L100" s="54">
-        <v>1006</v>
+      <c r="L100" s="5">
+        <v>1004</v>
       </c>
       <c r="M100" s="22" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="N100" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O100" s="55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O100" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B101" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D101" s="4">
-        <v>302</v>
+        <v>55</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>37</v>
@@ -27704,41 +27853,41 @@
         <v>40</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L101" s="5">
-        <v>1007</v>
+        <v>1015</v>
       </c>
       <c r="M101" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="N101" s="22" t="s">
         <v>42</v>
       </c>
       <c r="O101" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B102" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D102" s="4">
+      <c r="C102" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102" s="54">
         <v>302</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="F102" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G102" s="16">
+      <c r="G102" s="4">
         <v>403</v>
       </c>
       <c r="H102" s="35" t="s">
@@ -27747,34 +27896,34 @@
       <c r="I102" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J102" s="4" t="s">
+      <c r="J102" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K102" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L102" s="5">
-        <v>1008</v>
+        <v>51</v>
+      </c>
+      <c r="L102" s="54">
+        <v>1006</v>
       </c>
       <c r="M102" s="22" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="N102" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O102" s="22" t="s">
+      <c r="O102" s="55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B103" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="D103" s="4">
         <v>302</v>
@@ -27801,10 +27950,10 @@
         <v>47</v>
       </c>
       <c r="L103" s="5">
-        <v>5001</v>
+        <v>1007</v>
       </c>
       <c r="M103" s="22" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="N103" s="22" t="s">
         <v>42</v>
@@ -27813,15 +27962,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="31.5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B104" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>175</v>
+        <v>61</v>
       </c>
       <c r="D104" s="4">
         <v>302</v>
@@ -27845,127 +27994,127 @@
         <v>40</v>
       </c>
       <c r="K104" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L104" s="5">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="M104" s="22" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
       <c r="N104" s="22" t="s">
         <v>42</v>
       </c>
       <c r="O104" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="B105" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C105" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D105" s="16">
-        <v>305</v>
-      </c>
-      <c r="E105" s="16" t="s">
+      <c r="C105" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D105" s="4">
+        <v>302</v>
+      </c>
+      <c r="E105" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F105" s="16" t="s">
+      <c r="F105" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G105" s="26">
-        <v>400</v>
-      </c>
-      <c r="H105" s="4" t="s">
+      <c r="G105" s="16">
+        <v>403</v>
+      </c>
+      <c r="H105" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I105" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J105" s="16" t="s">
+      <c r="J105" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K105" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L105" s="17">
-        <v>1009</v>
-      </c>
-      <c r="M105" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="N105" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="O105" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" ht="63" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K105" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L105" s="5">
+        <v>5001</v>
+      </c>
+      <c r="M105" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="N105" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="O105" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="31.5" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="C106" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="D106" s="16">
-        <v>305</v>
-      </c>
-      <c r="E106" s="16" t="s">
+      <c r="C106" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D106" s="4">
+        <v>302</v>
+      </c>
+      <c r="E106" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F106" s="16" t="s">
+      <c r="F106" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G106" s="26">
-        <v>400</v>
-      </c>
-      <c r="H106" s="4" t="s">
+      <c r="G106" s="16">
+        <v>403</v>
+      </c>
+      <c r="H106" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I106" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J106" s="16" t="s">
+      <c r="J106" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K106" s="16" t="s">
-        <v>51</v>
+      <c r="K106" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="L106" s="5">
-        <v>3002</v>
-      </c>
-      <c r="M106" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="N106" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="O106" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" ht="47.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>1011</v>
+      </c>
+      <c r="M106" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="N106" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="O106" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="B107" s="57" t="s">
         <v>172</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D107" s="16" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="D107" s="16">
+        <v>305</v>
       </c>
       <c r="E107" s="16" t="s">
         <v>37</v>
@@ -27988,52 +28137,112 @@
       <c r="K107" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L107" s="18">
-        <v>3003</v>
+      <c r="L107" s="17">
+        <v>1009</v>
       </c>
       <c r="M107" s="23" t="s">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="N107" s="23" t="s">
         <v>176</v>
       </c>
       <c r="O107" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="63" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>112</v>
+      </c>
+      <c r="B108" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D108" s="16">
+        <v>305</v>
+      </c>
+      <c r="E108" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F108" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G108" s="26">
+        <v>400</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I108" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J108" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K108" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L108" s="5">
+        <v>3002</v>
+      </c>
+      <c r="M108" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="N108" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="O108" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="47.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>113</v>
+      </c>
+      <c r="B109" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F109" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G109" s="26">
+        <v>400</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I109" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J109" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K109" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L109" s="18">
+        <v>3003</v>
+      </c>
+      <c r="M109" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="N109" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="O109" s="23" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="12"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="12"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
-      <c r="J108" s="12"/>
-      <c r="K108" s="12"/>
-      <c r="L108" s="12"/>
-      <c r="M108" s="13"/>
-      <c r="N108" s="13"/>
-      <c r="O108" s="13"/>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
-      <c r="B109" s="13"/>
-      <c r="C109" s="52"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="12"/>
-      <c r="K109" s="12"/>
-      <c r="L109" s="12"/>
-      <c r="M109" s="13"/>
-      <c r="N109" s="13"/>
-      <c r="O109" s="13"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
@@ -31948,6 +32157,7 @@
     <row r="340" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A340" s="12"/>
       <c r="B340" s="13"/>
+      <c r="C340" s="52"/>
       <c r="D340" s="12"/>
       <c r="E340" s="12"/>
       <c r="F340" s="12"/>
@@ -31961,29 +32171,62 @@
       <c r="N340" s="13"/>
       <c r="O340" s="13"/>
     </row>
+    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A341" s="12"/>
+      <c r="B341" s="13"/>
+      <c r="C341" s="52"/>
+      <c r="D341" s="12"/>
+      <c r="E341" s="12"/>
+      <c r="F341" s="12"/>
+      <c r="G341" s="27"/>
+      <c r="H341" s="27"/>
+      <c r="I341" s="27"/>
+      <c r="J341" s="12"/>
+      <c r="K341" s="12"/>
+      <c r="L341" s="12"/>
+      <c r="M341" s="13"/>
+      <c r="N341" s="13"/>
+      <c r="O341" s="13"/>
+    </row>
+    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A342" s="12"/>
+      <c r="B342" s="13"/>
+      <c r="D342" s="12"/>
+      <c r="E342" s="12"/>
+      <c r="F342" s="12"/>
+      <c r="G342" s="27"/>
+      <c r="H342" s="27"/>
+      <c r="I342" s="27"/>
+      <c r="J342" s="12"/>
+      <c r="K342" s="12"/>
+      <c r="L342" s="12"/>
+      <c r="M342" s="13"/>
+      <c r="N342" s="13"/>
+      <c r="O342" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A61:O61"/>
+    <mergeCell ref="A62:O62"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
-    <mergeCell ref="A46:O46"/>
     <mergeCell ref="A47:O47"/>
-    <mergeCell ref="A92:O92"/>
-    <mergeCell ref="A93:O93"/>
-    <mergeCell ref="A76:O76"/>
-    <mergeCell ref="A62:O62"/>
+    <mergeCell ref="A48:O48"/>
+    <mergeCell ref="A94:O94"/>
+    <mergeCell ref="A95:O95"/>
     <mergeCell ref="A77:O77"/>
+    <mergeCell ref="A63:O63"/>
+    <mergeCell ref="A78:O78"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L56:L60 L11:L15 L71:L75 L23:L24 L31:L32 L17:L18 L7:L9 L67:L69 L52:L54 L26:L29 L85:L88 L91 L81:L83 L97:L99 L101:L106" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L57:L61 L11:L15 L72:L76 L23:L24 L31:L32 L17:L18 L7:L9 L68:L70 L53:L55 L26:L29 L86:L89 L103:L108 L82:L84 L99:L101 L92" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K56:K60 K71:K75 K67:K69 K7:K9 K52:K54 K11:K18 K85:K91 K81:K83 K101:K107 K97:K99 K23:K45" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K57:K61 K72:K76 K68:K70 K7:K9 K53:K55 K11:K18 K23:K45 K82:K84 K103:K109 K99:K101 K86:K93" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J56:J60 J71:J75 J67:J69 J7:J9 J52:J54 J11:J18 J85:J91 J81:J83 J101:J107 J97:J99 J23:J45" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J57:J61 J72:J76 J68:J70 J7:J9 J53:J55 J11:J18 J23:J45 J82:J84 J103:J109 J99:J101 J86:J93" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
       <formula1>"Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>
@@ -31993,67 +32236,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <UserInfo>
-        <DisplayName>Hunt, Martin</DisplayName>
-        <AccountId>118</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -32273,25 +32455,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <UserInfo>
+        <DisplayName>Hunt, Martin</DisplayName>
+        <AccountId>118</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32307,4 +32532,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>